<commit_message>
Updated schematic and PCB
Reduced the loop length to just over half the original length. Added more Vias for stitching. Changed MOSFET to handle up to 48V, meaning that the system can work up to 48V while still maintaining the 65A continuous rating.
</commit_message>
<xml_diff>
--- a/Buck 5V BOM.xlsx
+++ b/Buck 5V BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chanson\Desktop\Motor-Controller-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F27E5D2-AA13-4706-AF64-2C296FFFCC12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC0392D-E4C7-4609-8B95-D3EDA9272E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="3030" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3720" yWindow="3720" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -136,15 +136,6 @@
     <t>https://www.digikey.com/en/products/detail/cui-devices/DS04-254-2-03BK-SMT/11310920</t>
   </si>
   <si>
-    <t>IRF1404ZSTRLPBFCT-ND</t>
-  </si>
-  <si>
-    <t>N-Channel 40 V 180A (Tc) 200W (Tc) Surface Mount D²PAK (TO-263AB)</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/infineon-technologies/IRF1404ZSTRLPBF/1928315</t>
-  </si>
-  <si>
     <t>Connector Header Through Hole 5 position 0.100" (2.54mm)</t>
   </si>
   <si>
@@ -311,6 +302,15 @@
   </si>
   <si>
     <t>C10</t>
+  </si>
+  <si>
+    <t>IRFS3306TRLPBFCT-ND</t>
+  </si>
+  <si>
+    <t>N-Channel 60 V 120A (Tc) 230W (Tc) Surface Mount D2PAK</t>
+  </si>
+  <si>
+    <t>https://www.infineon.com/dgdl/irfs3306pbf.pdf?fileId=5546d462533600a40153563682652165</t>
   </si>
 </sst>
 </file>
@@ -916,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,7 +960,7 @@
     </row>
     <row r="2" spans="1:9" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>12</v>
@@ -987,13 +987,13 @@
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D3" s="12">
         <v>1</v>
@@ -1009,7 +1009,7 @@
         <v>0.73</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
@@ -1017,10 +1017,10 @@
         <v>20</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D4" s="12">
         <v>1</v>
@@ -1036,7 +1036,7 @@
         <v>2.56</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
@@ -1044,10 +1044,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D5" s="12">
         <v>1</v>
@@ -1063,18 +1063,18 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D6" s="20">
         <v>1</v>
@@ -1090,18 +1090,18 @@
         <v>0.49</v>
       </c>
       <c r="H6" s="22" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D7" s="20">
         <v>2</v>
@@ -1117,34 +1117,34 @@
         <v>0.6</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>32</v>
+        <v>88</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="D8" s="20">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E8" s="21">
-        <v>1.91</v>
+        <v>2.58</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>7</v>
       </c>
       <c r="G8" s="19">
         <f t="shared" si="0"/>
-        <v>15.28</v>
+        <v>10.32</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1152,10 +1152,10 @@
         <v>10</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D9" s="20">
         <v>1</v>
@@ -1171,7 +1171,7 @@
         <v>1.64</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I9" s="17"/>
     </row>
@@ -1180,10 +1180,10 @@
         <v>11</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D10" s="20">
         <v>1</v>
@@ -1199,18 +1199,18 @@
         <v>2.27</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D11" s="20">
         <v>1</v>
@@ -1229,13 +1229,13 @@
     </row>
     <row r="12" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D12" s="20">
         <v>1</v>
@@ -1251,18 +1251,18 @@
         <v>0.52</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D13" s="20">
         <v>4</v>
@@ -1278,7 +1278,7 @@
         <v>1.4</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1305,7 +1305,7 @@
         <v>18.36</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
@@ -1313,10 +1313,10 @@
         <v>16</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D15" s="12">
         <v>1</v>
@@ -1332,18 +1332,18 @@
         <v>1.43</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D16" s="12">
         <v>1</v>
@@ -1359,18 +1359,18 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D17" s="12">
         <v>9</v>
@@ -1386,7 +1386,7 @@
         <v>3.5100000000000002</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
@@ -1421,7 +1421,7 @@
         <v>21</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C19" s="16" t="s">
         <v>23</v>
@@ -1440,7 +1440,7 @@
         <v>2.7</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="36.75" x14ac:dyDescent="0.25">
@@ -1473,10 +1473,10 @@
         <v>22</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D21" s="13">
         <v>4</v>
@@ -1492,7 +1492,7 @@
         <v>1.64</v>
       </c>
       <c r="H21" s="22" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.3">
@@ -1500,7 +1500,7 @@
         <v>14</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>19</v>
@@ -1519,7 +1519,7 @@
         <v>0.97</v>
       </c>
       <c r="H22" s="29" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1528,7 +1528,7 @@
       </c>
       <c r="G23" s="7">
         <f>SUM(G2:G22)</f>
-        <v>61.419999999999995</v>
+        <v>56.46</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1592,23 +1592,23 @@
     <hyperlink ref="H2" r:id="rId1" xr:uid="{EC06BA25-5BBF-4256-803F-A9FDB457E9B1}"/>
     <hyperlink ref="H20" r:id="rId2" xr:uid="{AC81996F-D568-4668-86FA-D435AC539FA0}"/>
     <hyperlink ref="H18" r:id="rId3" xr:uid="{824F3F0F-8998-4AED-93DD-622B79B65A28}"/>
-    <hyperlink ref="H8" r:id="rId4" xr:uid="{FEA59C81-A7B8-4225-9F47-3AFC30030BA9}"/>
-    <hyperlink ref="H15" r:id="rId5" xr:uid="{C7647B1F-5AC7-476C-92B6-E61230E0D1CD}"/>
-    <hyperlink ref="H16" r:id="rId6" xr:uid="{6D4EA0A2-CFDF-4E3D-9F0E-96E89FBB0A78}"/>
-    <hyperlink ref="H17" r:id="rId7" xr:uid="{915E4EB1-02CF-4478-8AAD-416A6829D2AF}"/>
-    <hyperlink ref="H21" r:id="rId8" xr:uid="{BFC3512A-DC63-45F2-9FF7-B4E26C9381EA}"/>
-    <hyperlink ref="H9" r:id="rId9" xr:uid="{EC517467-96DF-4B7B-AA7B-7290FF844D5E}"/>
-    <hyperlink ref="H22" r:id="rId10" xr:uid="{A8BA41E3-0DB9-477E-9511-169BFBF38909}"/>
-    <hyperlink ref="H19" r:id="rId11" xr:uid="{9B76D1D7-DAF2-447F-AF48-0C187821D5C5}"/>
-    <hyperlink ref="H14" r:id="rId12" xr:uid="{B98F2375-85D1-43B3-B952-25B29C8270AC}"/>
-    <hyperlink ref="H5" r:id="rId13" xr:uid="{8CAB2C01-8D57-4F1A-A16C-ED1684128666}"/>
-    <hyperlink ref="H7" r:id="rId14" xr:uid="{6E7AD1B6-E187-452B-A2D5-F611418D3F75}"/>
-    <hyperlink ref="H4" r:id="rId15" xr:uid="{2BE8EB22-9255-4BDC-ACF3-9DC6D095A159}"/>
-    <hyperlink ref="H6" r:id="rId16" xr:uid="{BC4186EC-63DB-4284-A0BA-CD20D91CD4DD}"/>
-    <hyperlink ref="H10" r:id="rId17" xr:uid="{E12F43D3-7B18-48D2-B45D-871208E6E28C}"/>
-    <hyperlink ref="H12" r:id="rId18" xr:uid="{2D6C0A81-1EC9-4FA5-BCBA-23C407663010}"/>
-    <hyperlink ref="H13" r:id="rId19" xr:uid="{28A63484-4740-4D85-A1B3-E119463E6BD6}"/>
-    <hyperlink ref="H3" r:id="rId20" xr:uid="{FD5D0C32-AD08-46C3-BC7F-C3B51DF6FD14}"/>
+    <hyperlink ref="H15" r:id="rId4" xr:uid="{C7647B1F-5AC7-476C-92B6-E61230E0D1CD}"/>
+    <hyperlink ref="H16" r:id="rId5" xr:uid="{6D4EA0A2-CFDF-4E3D-9F0E-96E89FBB0A78}"/>
+    <hyperlink ref="H17" r:id="rId6" xr:uid="{915E4EB1-02CF-4478-8AAD-416A6829D2AF}"/>
+    <hyperlink ref="H21" r:id="rId7" xr:uid="{BFC3512A-DC63-45F2-9FF7-B4E26C9381EA}"/>
+    <hyperlink ref="H9" r:id="rId8" xr:uid="{EC517467-96DF-4B7B-AA7B-7290FF844D5E}"/>
+    <hyperlink ref="H22" r:id="rId9" xr:uid="{A8BA41E3-0DB9-477E-9511-169BFBF38909}"/>
+    <hyperlink ref="H19" r:id="rId10" xr:uid="{9B76D1D7-DAF2-447F-AF48-0C187821D5C5}"/>
+    <hyperlink ref="H14" r:id="rId11" xr:uid="{B98F2375-85D1-43B3-B952-25B29C8270AC}"/>
+    <hyperlink ref="H5" r:id="rId12" xr:uid="{8CAB2C01-8D57-4F1A-A16C-ED1684128666}"/>
+    <hyperlink ref="H7" r:id="rId13" xr:uid="{6E7AD1B6-E187-452B-A2D5-F611418D3F75}"/>
+    <hyperlink ref="H4" r:id="rId14" xr:uid="{2BE8EB22-9255-4BDC-ACF3-9DC6D095A159}"/>
+    <hyperlink ref="H6" r:id="rId15" xr:uid="{BC4186EC-63DB-4284-A0BA-CD20D91CD4DD}"/>
+    <hyperlink ref="H10" r:id="rId16" xr:uid="{E12F43D3-7B18-48D2-B45D-871208E6E28C}"/>
+    <hyperlink ref="H12" r:id="rId17" xr:uid="{2D6C0A81-1EC9-4FA5-BCBA-23C407663010}"/>
+    <hyperlink ref="H13" r:id="rId18" xr:uid="{28A63484-4740-4D85-A1B3-E119463E6BD6}"/>
+    <hyperlink ref="H3" r:id="rId19" xr:uid="{FD5D0C32-AD08-46C3-BC7F-C3B51DF6FD14}"/>
+    <hyperlink ref="H8" r:id="rId20" xr:uid="{E32EE017-42E4-4CF2-9F0F-93BCABEB36A9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Parts to match what was bought
</commit_message>
<xml_diff>
--- a/Buck 5V BOM.xlsx
+++ b/Buck 5V BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chanson\Desktop\Motor-Controller-main\Motor-Controller-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chanson\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEFE6AA-F6AA-4E83-882B-F2E0679AEB28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45562C58-49EA-4600-B00A-EBF91448B0F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -244,15 +244,6 @@
     <t>https://www.infineon.com/dgdl/irfs3306pbf.pdf?fileId=5546d462533600a40153563682652165</t>
   </si>
   <si>
-    <t>175-MAX17640CATA+-ND</t>
-  </si>
-  <si>
-    <t>Buck Switching Regulator IC Positive Adjustable 0.9V 1 Output 400mA 8-WDFN</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/maxim-integrated/MAX17640CATA/14287861</t>
-  </si>
-  <si>
     <t>Q1-Q4</t>
   </si>
   <si>
@@ -338,6 +329,15 @@
   </si>
   <si>
     <t>Red, Yellow 630nm Red, 591nm Yellow LED Indication - Discrete 2V Red, 2V Yellow 0603 (1608 Metric)</t>
+  </si>
+  <si>
+    <t>175-MAX17640BATA+-ND</t>
+  </si>
+  <si>
+    <t>Buck Switching Regulator IC Positive Fixed 5V 1 Output 400mA 8-WFDFN</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/maxim-integrated/MAX17640BATA/14287859?s=N4IgTCBcDaIIwHYCsBaAsgQQBqIGwBYAGAIQwBUMBqFAOQBEQBdAXyA</t>
   </si>
 </sst>
 </file>
@@ -944,8 +944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,13 +988,13 @@
     </row>
     <row r="2" spans="1:9" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D2" s="12">
         <v>4</v>
@@ -1015,7 +1015,7 @@
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>62</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="4" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D4" s="12">
         <v>2</v>
@@ -1064,7 +1064,7 @@
         <v>5.84</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1096,7 +1096,7 @@
     </row>
     <row r="6" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>51</v>
@@ -1123,13 +1123,13 @@
     </row>
     <row r="7" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D7" s="20">
         <v>1</v>
@@ -1145,18 +1145,18 @@
         <v>0.37</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>96</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>99</v>
       </c>
       <c r="D8" s="20">
         <v>1</v>
@@ -1172,18 +1172,18 @@
         <v>0.43</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D9" s="20">
         <v>2</v>
@@ -1199,12 +1199,12 @@
         <v>0.2</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>65</v>
@@ -1257,15 +1257,15 @@
       </c>
       <c r="I11" s="17"/>
     </row>
-    <row r="12" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>68</v>
+        <v>97</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="D12" s="20">
         <v>1</v>
@@ -1281,7 +1281,7 @@
         <v>1.65</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
@@ -1289,10 +1289,10 @@
         <v>58</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D13" s="20">
         <v>1</v>
@@ -1308,7 +1308,7 @@
         <v>0.3</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
@@ -1316,10 +1316,10 @@
         <v>54</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D14" s="20">
         <v>1</v>
@@ -1335,12 +1335,12 @@
         <v>0.71</v>
       </c>
       <c r="H14" s="31" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>59</v>
@@ -1554,7 +1554,7 @@
     </row>
     <row r="23" spans="1:8" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>40</v>
@@ -1689,13 +1689,13 @@
     <hyperlink ref="H15" r:id="rId14" xr:uid="{28A63484-4740-4D85-A1B3-E119463E6BD6}"/>
     <hyperlink ref="H3" r:id="rId15" xr:uid="{FD5D0C32-AD08-46C3-BC7F-C3B51DF6FD14}"/>
     <hyperlink ref="H10" r:id="rId16" xr:uid="{E32EE017-42E4-4CF2-9F0F-93BCABEB36A9}"/>
-    <hyperlink ref="H12" r:id="rId17" xr:uid="{0FC6BF4E-B3F7-4B10-8F3D-F4990499FCDC}"/>
-    <hyperlink ref="H13" r:id="rId18" xr:uid="{5B927924-9F42-4FC1-A54D-3FA96B6BE0F8}"/>
-    <hyperlink ref="H14" r:id="rId19" display="https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL32B226MOJVPNE/11487778" xr:uid="{261B60BF-E7B9-412E-ADE9-39C9C22F5694}"/>
-    <hyperlink ref="H4" r:id="rId20" xr:uid="{A3B9EFD3-1AE1-432D-A046-EB69FFDD8413}"/>
-    <hyperlink ref="H7" r:id="rId21" xr:uid="{A8C64BFE-52FE-4913-BF99-4ABD728FEB84}"/>
-    <hyperlink ref="H9" r:id="rId22" xr:uid="{866C3AA0-47E7-4D34-B47F-E2C9626259D5}"/>
-    <hyperlink ref="H8" r:id="rId23" xr:uid="{42BC71AF-2E36-45CB-9A55-C1B1ECA63DD6}"/>
+    <hyperlink ref="H13" r:id="rId17" xr:uid="{5B927924-9F42-4FC1-A54D-3FA96B6BE0F8}"/>
+    <hyperlink ref="H14" r:id="rId18" display="https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL32B226MOJVPNE/11487778" xr:uid="{261B60BF-E7B9-412E-ADE9-39C9C22F5694}"/>
+    <hyperlink ref="H4" r:id="rId19" xr:uid="{A3B9EFD3-1AE1-432D-A046-EB69FFDD8413}"/>
+    <hyperlink ref="H7" r:id="rId20" xr:uid="{A8C64BFE-52FE-4913-BF99-4ABD728FEB84}"/>
+    <hyperlink ref="H9" r:id="rId21" xr:uid="{866C3AA0-47E7-4D34-B47F-E2C9626259D5}"/>
+    <hyperlink ref="H8" r:id="rId22" xr:uid="{42BC71AF-2E36-45CB-9A55-C1B1ECA63DD6}"/>
+    <hyperlink ref="H12" r:id="rId23" xr:uid="{10D4338B-26FF-4D3A-B8B8-B02388C4D37D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId24"/>

</xml_diff>